<commit_message>
PLP and Parallel Projects updated for all batches
</commit_message>
<xml_diff>
--- a/1st_August_Batch_Java_Full_Stack/MPT_MTT/Module 1/JavaFullStack-Module1_Java_SQL_DB_JDBC_MTT-Assessment_revised.xlsx
+++ b/1st_August_Batch_Java_Full_Stack/MPT_MTT/Module 1/JavaFullStack-Module1_Java_SQL_DB_JDBC_MTT-Assessment_revised.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit\Desktop\Caps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Company\CG\JSpiders-CG-HTDProgram\1st_August_Batch_Java_Full_Stack\MPT_MTT\Module 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1009,7 +1009,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -1673,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>